<commit_message>
testing cs42448 codec and audio fx routing
</commit_message>
<xml_diff>
--- a/Order2.xlsx
+++ b/Order2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arvid\Documents\PlatformIO\Projects\HEX_DSP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8104345-C6EB-4E25-88CD-D14DA9B92E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1006C5-49FF-438F-8ED8-49F0ADA43909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FCDD146C-BDB8-4F9C-A827-12FA43291FA4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FCDD146C-BDB8-4F9C-A827-12FA43291FA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>https://www.electrokit.com/rotationsenkoder-24-p/v-med-tryckknapp-fasta-lagen</t>
   </si>
@@ -50,12 +50,6 @@
     <t>Ratt gummi svart ø16x14.7mm D-axel</t>
   </si>
   <si>
-    <t>https://www.electrokit.com/d-sub-15-pol-hd-hona</t>
-  </si>
-  <si>
-    <t>D-SUB 15 pol HD hona</t>
-  </si>
-  <si>
     <t>Amount</t>
   </si>
   <si>
@@ -63,6 +57,24 @@
   </si>
   <si>
     <t>link</t>
+  </si>
+  <si>
+    <t>https://www.electrokit.com/lcd-tft-2.8touch-ili9341</t>
+  </si>
+  <si>
+    <t>LCD TFT 2.8" touch (ILI9341)</t>
+  </si>
+  <si>
+    <t>https://www.electrokit.com/6.3mm-chassie-mono-med-brytare</t>
+  </si>
+  <si>
+    <t>6.3mm hona 2-pol mono chassie brytare</t>
+  </si>
+  <si>
+    <t>https://www.electrokit.com/d-sub-15-pol-hd-hona-pcb</t>
+  </si>
+  <si>
+    <t>D-SUB 15 pol HD hona PCB</t>
   </si>
 </sst>
 </file>
@@ -445,7 +457,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC5BBC6B-1C15-4B44-8E22-A517AB0CDF52}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
@@ -458,13 +470,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -491,20 +503,43 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{0BE97022-E08A-4D4E-A818-4F262C523243}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{47EC4621-D1E9-4E3F-95E7-817DC7CA228B}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{081A5B49-7D49-49D4-82C3-98BF50D1D24C}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{654C3F5E-5B4F-4709-8EDD-968E22230B86}"/>
+    <hyperlink ref="D6" r:id="rId4" xr:uid="{CA341D9F-E2D0-492D-A823-3A3C3F61FDB1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>